<commit_message>
Initial version with virtual environment setup
</commit_message>
<xml_diff>
--- a/Ratios de Inversion 2024.xlsx
+++ b/Ratios de Inversion 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stocks_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2F9FEB-1834-48D0-8B94-13F67D2BDCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387DC4FB-0717-49C3-9BAB-5A37783621DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios de Inversión" sheetId="1" r:id="rId1"/>
@@ -992,19 +992,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" customWidth="1"/>
+    <col min="3" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="37.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1040,7 +1040,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1089,7 +1089,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>17</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1156,7 +1156,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1186,7 +1186,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1227,7 +1227,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>28</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="23" t="s">
         <v>29</v>
@@ -1253,7 +1253,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
@@ -1264,7 +1264,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
@@ -1275,7 +1275,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -1286,7 +1286,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="23" t="s">
         <v>30</v>
@@ -1311,7 +1311,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="7.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -1320,7 +1320,7 @@
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
     </row>
-    <row r="21" spans="1:9" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -1329,7 +1329,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
     </row>
-    <row r="22" spans="1:9" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1338,7 +1338,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="29" t="s">
         <v>31</v>
       </c>
@@ -1359,24 +1359,24 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B32" s="11"/>
     </row>
   </sheetData>
@@ -1422,12 +1422,12 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1443,17 +1443,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>39</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>39.118931925805022</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>40</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>34.217428831851997</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>41</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>12.326716997933749</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>42</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>15.625241739943499</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>43</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>19.917364293472431</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>44</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>35.947868357962491</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>45</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>10.62613375303453</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>46</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>15.85127930786226</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>47</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>20.19414147634847</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>48</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>28.205949186612312</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>49</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>9.9339651137367273</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>50</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>32.026370366400933</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>51</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>18.902089424170171</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>26.441089562859819</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>53</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>11.984361832564259</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>54</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>16.73928063049123</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>55</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>20.630037214247739</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>56</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>18.715106884222699</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>57</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>29.017205350531459</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>58</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>22.539145721072011</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>59</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>24.15185687872021</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>60</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>22.289626040495349</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>61</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>27.080318238837449</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>62</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>73.1985069471001</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>63</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>23.219719287748351</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>64</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>98.115107314515171</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>65</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>23.534849955101588</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>66</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>32.074018007042469</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>67</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>26.790993485412681</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
         <v>68</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>33.426337924371637</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>69</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>37.934845938964898</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>70</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>36.55581235716992</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>71</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>22.947007336466019</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>72</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>28.554239867188532</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>73</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>24.451496849891221</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
         <v>74</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>19.13346606850379</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>75</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>32.723816577810197</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>76</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>27.557960785908961</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
         <v>77</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>42.471016661824351</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
         <v>78</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>74.520471436559546</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>79</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>133.33079865476029</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>80</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>12.07434267949532</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>81</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>26.003626840539251</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>82</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>30.872329430832831</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
         <v>83</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>21.23842761890231</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
         <v>84</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>27.863828251821719</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
         <v>85</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>24.341000586407819</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
         <v>86</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>8.3789517181019075</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
         <v>87</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>17.03691875164991</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
         <v>88</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>26.790016253414311</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
         <v>89</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>27.294408069917299</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
         <v>90</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>68.67769194362613</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
         <v>91</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>15.527618107238</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
         <v>92</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>11.69738695057797</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="12" t="s">
         <v>93</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
         <v>94</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>14.19875936891523</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
         <v>95</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>13.960247471406641</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
         <v>96</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>14.7056130261956</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
         <v>97</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>11.755876983980389</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
         <v>98</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>15.71871389702199</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
         <v>99</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>61.081022099864541</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
         <v>100</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>18.6978223743039</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="12" t="s">
         <v>101</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>41.857527279353683</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
         <v>102</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>7.9275811209439526</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="12" t="s">
         <v>103</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>105.792987012987</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
         <v>104</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>49.111423935993187</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>105</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>16.87642636292772</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
         <v>106</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>8.5597883597883602</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>107</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>45.154979492672886</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
         <v>108</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>15.868785301601649</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="12" t="s">
         <v>109</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>23.194797092367001</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>110</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>28.28885131191916</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
         <v>111</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>20.228167060259821</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="13" t="s">
         <v>112</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>16.660716918810468</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
         <v>113</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>110.18394298945201</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
         <v>114</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>23.350926240004561</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
         <v>115</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>11.2755905511811</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="13" t="s">
         <v>116</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>45.770367963048542</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
         <v>117</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>28.833253120451388</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="13" t="s">
         <v>118</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>14.09265161277208</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
         <v>119</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>17.34800073725858</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="13" t="s">
         <v>120</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>45.964186869907827</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">
         <v>121</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>56.450797181267873</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="13" t="s">
         <v>122</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>56.925187317987607</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
         <v>123</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>24.409999133170931</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
         <v>124</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>25.641295352220379</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
         <v>125</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>23.19915230277239</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="13" t="s">
         <v>126</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>99.862558271942689</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
         <v>127</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>21.73709990062514</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="13" t="s">
         <v>128</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>30.918693672686889</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
         <v>129</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>19.816428600521341</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="13" t="s">
         <v>130</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>22.97608167201917</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
         <v>131</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>16.406976720204881</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="13" t="s">
         <v>132</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>25.373790321219381</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="12" t="s">
         <v>133</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>31.976432665788469</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="14" t="s">
         <v>134</v>
       </c>

</xml_diff>